<commit_message>
Init project, remove sampled data
</commit_message>
<xml_diff>
--- a/data/gdl_settings.xlsx
+++ b/data/gdl_settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/GeoPressureTemplate/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Library/CloudStorage/Box-Box/PAM_mongolia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C26FC5B-C776-8946-8F43-97A00E9B3653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718E57E5-CCE5-C74D-BDD7-7E396110C5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,17 +31,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Color</t>
   </si>
   <si>
+    <t>Eurasian Nightjar</t>
+  </si>
+  <si>
+    <t>22BT</t>
+  </si>
+  <si>
     <t>mass</t>
   </si>
   <si>
     <t>RingNo</t>
   </si>
   <si>
+    <t>include</t>
+  </si>
+  <si>
     <t>gdl_id</t>
   </si>
   <si>
@@ -114,23 +123,26 @@
     <t>prob_map_thr</t>
   </si>
   <si>
+    <t>22BS</t>
+  </si>
+  <si>
+    <t>24FD</t>
+  </si>
+  <si>
     <t>prob_light_w</t>
   </si>
   <si>
     <t>thr_dur</t>
-  </si>
-  <si>
-    <t>18LX</t>
-  </si>
-  <si>
-    <t>Great Reed Warbler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,11 +294,6 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFAD0000"/>
-      <name val="Var(--bs-font-monospace)"/>
     </font>
   </fonts>
   <fills count="33">
@@ -631,13 +638,15 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -686,16 +695,13 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
@@ -714,6 +720,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -763,13 +772,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AC2" totalsRowShown="0">
-  <autoFilter ref="A1:AC2" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
-  <tableColumns count="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AD4" totalsRowShown="0">
+  <autoFilter ref="A1:AD4" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+  <tableColumns count="30">
+    <tableColumn id="1" xr3:uid="{0C755099-5A61-5948-A224-A3E024CA3BDE}" name="include"/>
     <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="10" dataCellStyle="Normal_Feuil1"/>
     <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start"/>
     <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end"/>
-    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="9"/>
     <tableColumn id="43" xr3:uid="{0ACC25F8-5611-FA4F-B49C-6E30F1D95C08}" name="extent_N"/>
     <tableColumn id="44" xr3:uid="{7341665D-D68F-3E48-95CE-8E270ED9FA6A}" name="extent_W"/>
     <tableColumn id="45" xr3:uid="{18F1D038-2D60-FF49-8711-16897DCC1A1A}" name="extent_S"/>
@@ -779,17 +789,19 @@
     <tableColumn id="49" xr3:uid="{A0BE4E97-52EA-C245-B384-C2C954FDB62B}" name="map_margin"/>
     <tableColumn id="50" xr3:uid="{98646B4B-4B26-0A4C-A7C3-1140DBCABB7B}" name="prob_map_s"/>
     <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr"/>
-    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="9"/>
+    <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="8">
+      <calculatedColumnFormula>6*60*60</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon"/>
     <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="8"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="7"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="5"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="4"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="3"/>
     <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="0"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="RingNo" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="RingNo" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
@@ -1097,194 +1109,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA12" sqref="N12:AA12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.1640625" customWidth="1"/>
-    <col min="20" max="20" width="14.1640625" customWidth="1"/>
-    <col min="21" max="23" width="17.33203125" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5" customWidth="1"/>
-    <col min="33" max="33" width="16.33203125" customWidth="1"/>
-    <col min="39" max="41" width="15.1640625" customWidth="1"/>
-    <col min="42" max="42" width="14.5" customWidth="1"/>
-    <col min="43" max="43" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" customWidth="1"/>
+    <col min="22" max="24" width="17.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" customWidth="1"/>
+    <col min="27" max="27" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5" customWidth="1"/>
+    <col min="34" max="34" width="16.33203125" customWidth="1"/>
+    <col min="40" max="42" width="15.1640625" customWidth="1"/>
+    <col min="43" max="43" width="14.5" customWidth="1"/>
+    <col min="44" max="44" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="T1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="U1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="V1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="W1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="X1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="Y1" t="s">
         <v>4</v>
       </c>
       <c r="Z1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AA1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" t="b">
         <v>1</v>
       </c>
-      <c r="AB1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1">
-        <v>42906</v>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>43222</v>
-      </c>
-      <c r="D2" s="4">
-        <v>12</v>
-      </c>
-      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>73051</v>
+      </c>
+      <c r="E2" s="7">
+        <v>24</v>
+      </c>
+      <c r="F2">
         <v>50</v>
       </c>
-      <c r="F2">
-        <v>-16</v>
-      </c>
       <c r="G2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H2">
-        <v>23</v>
+        <v>-35</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <v>300</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>30</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.9</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
       <c r="O2">
-        <v>17.05</v>
+        <f t="shared" ref="O2:O4" si="0">6*60*60</f>
+        <v>21600</v>
       </c>
       <c r="P2">
-        <v>48.9</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>42906</v>
+        <v>110.83</v>
+      </c>
+      <c r="Q2">
+        <v>48.57</v>
       </c>
       <c r="R2" s="1">
-        <v>42952</v>
-      </c>
-      <c r="S2" s="1"/>
+        <v>43296</v>
+      </c>
+      <c r="S2" s="1">
+        <v>43338</v>
+      </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
-      <c r="W2" s="4">
+      <c r="W2" s="1"/>
+      <c r="X2" s="6">
         <v>0.1</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="2"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="2"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>73051</v>
+      </c>
+      <c r="E3" s="7">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>-35</v>
+      </c>
+      <c r="I3">
+        <v>120</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>300</v>
+      </c>
+      <c r="L3">
+        <v>30</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>21600</v>
+      </c>
+      <c r="P3">
+        <v>110.83</v>
+      </c>
+      <c r="Q3">
+        <v>48.57</v>
+      </c>
+      <c r="R3" s="1">
+        <v>43296</v>
+      </c>
+      <c r="S3" s="1">
+        <v>43331</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
     </row>
-    <row r="8" spans="1:29">
-      <c r="P8" s="3"/>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>73051</v>
+      </c>
+      <c r="E4" s="7">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>-35</v>
+      </c>
+      <c r="I4">
+        <v>120</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>300</v>
+      </c>
+      <c r="L4">
+        <v>30</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0.9</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>21600</v>
+      </c>
+      <c r="P4" s="3">
+        <v>110.69</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>48.59</v>
+      </c>
+      <c r="R4" s="1">
+        <v>43634.21875</v>
+      </c>
+      <c r="S4" s="1">
+        <v>43687.524305555555</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
     </row>
-    <row r="13" spans="1:29">
-      <c r="H13" s="5"/>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="Q10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>